<commit_message>
#1 Update documentation with 2 new test cases
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - Login.xlsx
+++ b/TestCases/Test Cases - Login.xlsx
@@ -5,27 +5,33 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geral\Desktop\ETI CA1.2\ETIToDoList\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633DD7C2-BDFE-4698-807D-B638AC3D34BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B07AEA-53A2-4461-81A4-F24AAAE70651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -136,6 +142,24 @@
     <t>Input:
 Username: "admin?"
 Password: "admin123"</t>
+  </si>
+  <si>
+    <t>The user will be brought to the login page.</t>
+  </si>
+  <si>
+    <t>To test if the login page can be navigated to successfully.</t>
+  </si>
+  <si>
+    <t>Test logout</t>
+  </si>
+  <si>
+    <t>Test navigation to login page</t>
+  </si>
+  <si>
+    <t>To check if user is able to logout.</t>
+  </si>
+  <si>
+    <t>The user will be brought to the logged out page.</t>
   </si>
 </sst>
 </file>
@@ -203,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -218,9 +242,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -508,23 +529,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:G7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.17578125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="4.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="44.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.1796875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="58.7265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="27.7265625" style="3" customWidth="1"/>
-    <col min="6" max="7" width="17.453125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.26953125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="4.46875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="44.8203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.17578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="58.703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.703125" style="3" customWidth="1"/>
+    <col min="6" max="7" width="17.46875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.29296875" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.17578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -547,7 +568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -570,7 +591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="5">
         <v>1.1000000000000001</v>
       </c>
@@ -593,7 +614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="5">
         <v>1.2</v>
       </c>
@@ -616,7 +637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="5">
         <v>1.3</v>
       </c>
@@ -639,7 +660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="5">
         <v>1.4</v>
       </c>
@@ -662,7 +683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="5">
         <v>1.5</v>
       </c>
@@ -685,46 +706,74 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="13" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#6 Updated test outputs and Test Cases - Login.xlsx
Finished testing, updated the test outputs and the test case excel sheet (Test Cases - Login.xlsx)
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - Login.xlsx
+++ b/TestCases/Test Cases - Login.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\ETI_ToDoList\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B07AEA-53A2-4461-81A4-F24AAAE70651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE06EFA-FF12-44CF-BBFA-3B5A90A941C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Fail/Pass</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>The user will be brought to the logged out page.</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -529,25 +529,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.17578125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.46875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="44.8203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.17578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="58.703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="27.703125" style="3" customWidth="1"/>
-    <col min="6" max="7" width="17.46875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.29296875" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.17578125" style="3"/>
+    <col min="1" max="1" width="4.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="44.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.1796875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="58.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.7265625" style="3" customWidth="1"/>
+    <col min="6" max="7" width="17.453125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -568,191 +568,191 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>1.2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>1.3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>1.4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>1.5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>1.6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>1.7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -761,7 +761,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -770,10 +770,10 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="13" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="12" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#1 added new login test cases
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - Login.xlsx
+++ b/TestCases/Test Cases - Login.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI-ToDoList (GitHub)\ETI_ToDoList\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B07AEA-53A2-4461-81A4-F24AAAE70651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAF678B-DFF4-422A-B647-EA21EA73D243}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Fail/Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>-</t>
@@ -160,6 +157,36 @@
   </si>
   <si>
     <t>The user will be brought to the logged out page.</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Test successful login from backend</t>
+  </si>
+  <si>
+    <t>Test login with incorrect username from backend</t>
+  </si>
+  <si>
+    <t>Test login with incorrect password from backend</t>
+  </si>
+  <si>
+    <t>To check if an invalid user with an invalid username can log in by calling the method for login and passing in the login credentials.</t>
+  </si>
+  <si>
+    <t>To check if a valid user can log in by calling the method for login and passing in the login credentials.</t>
+  </si>
+  <si>
+    <t>To check if an valid user with an invalid password can log in by calling the method for login and passing in the login credentials.</t>
+  </si>
+  <si>
+    <t>The user is authenticated and logged in successfully.</t>
+  </si>
+  <si>
+    <t>The user is not authenticated and unable to login.</t>
   </si>
 </sst>
 </file>
@@ -227,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -242,9 +269,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -530,24 +554,24 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.17578125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.46875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="44.8203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.17578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="58.703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="27.703125" style="3" customWidth="1"/>
-    <col min="6" max="7" width="17.46875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.29296875" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.17578125" style="3"/>
+    <col min="1" max="1" width="4.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="58.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" style="3" customWidth="1"/>
+    <col min="6" max="7" width="17.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -568,212 +592,262 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1.2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1.3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>1.4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>1.5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1.6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>1.7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="13" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.5"/>
+    </row>
+    <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#6 Updated Test Cases - Login.xlsx and test outputs
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - Login.xlsx
+++ b/TestCases/Test Cases - Login.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI-ToDoList (GitHub)\ETI_ToDoList\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\ETI_ToDoList\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAF678B-DFF4-422A-B647-EA21EA73D243}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF1F172-3DB4-4B7F-892C-2801B5F37FB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -162,9 +162,6 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t>Test successful login from backend</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>The user is not authenticated and unable to login.</t>
+  </si>
+  <si>
+    <t>Same as expected outcome.</t>
   </si>
 </sst>
 </file>
@@ -553,23 +553,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" style="3" customWidth="1"/>
-    <col min="6" max="7" width="17.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="4.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="44.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.1796875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="58.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.7265625" style="3" customWidth="1"/>
+    <col min="6" max="7" width="17.453125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -592,7 +592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -609,13 +609,13 @@
         <v>16</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1.1000000000000001</v>
       </c>
@@ -632,13 +632,13 @@
         <v>17</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>1.2</v>
       </c>
@@ -655,13 +655,13 @@
         <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>1.3</v>
       </c>
@@ -678,13 +678,13 @@
         <v>19</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>1.4</v>
       </c>
@@ -701,13 +701,13 @@
         <v>20</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>1.5</v>
       </c>
@@ -724,13 +724,13 @@
         <v>21</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>1.6</v>
       </c>
@@ -747,13 +747,13 @@
         <v>32</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>1.7</v>
       </c>
@@ -770,84 +770,84 @@
         <v>37</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>1.8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>1.9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>2</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added justifications if any column to test cases
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - Login.xlsx
+++ b/TestCases/Test Cases - Login.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\ETI_ToDoList\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\test master 5\ETI_ToDoList\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF1F172-3DB4-4B7F-892C-2801B5F37FB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905C711B-7032-4251-98FF-2246966189C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="49">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Same as expected outcome.</t>
+  </si>
+  <si>
+    <t>Justifications (if any)</t>
   </si>
 </sst>
 </file>
@@ -551,25 +554,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="44.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.1796875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="58.7265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="27.7265625" style="3" customWidth="1"/>
-    <col min="6" max="7" width="17.453125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.26953125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="4.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="58.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" style="3" customWidth="1"/>
+    <col min="6" max="7" width="17.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -591,8 +594,11 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -614,8 +620,11 @@
       <c r="G2" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1.1000000000000001</v>
       </c>
@@ -637,8 +646,11 @@
       <c r="G3" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1.2</v>
       </c>
@@ -660,8 +672,11 @@
       <c r="G4" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1.3</v>
       </c>
@@ -683,8 +698,11 @@
       <c r="G5" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>1.4</v>
       </c>
@@ -706,8 +724,11 @@
       <c r="G6" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H6" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>1.5</v>
       </c>
@@ -729,8 +750,11 @@
       <c r="G7" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H7" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1.6</v>
       </c>
@@ -752,8 +776,11 @@
       <c r="G8" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H8" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>1.7</v>
       </c>
@@ -775,8 +802,11 @@
       <c r="G9" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H9" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>1.8</v>
       </c>
@@ -798,8 +828,11 @@
       <c r="G10" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H10" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>1.9</v>
       </c>
@@ -821,8 +854,11 @@
       <c r="G11" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H11" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2</v>
       </c>
@@ -844,10 +880,13 @@
       <c r="G12" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="H12" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>